<commit_message>
use blog website not github landing  page
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profils\mcanouil\PROJECTS\mc-curriculum_vitae\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profils\mcanouil\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -688,9 +688,6 @@
     <t>website</t>
   </si>
   <si>
-    <t>https://m.canouil.fr/</t>
-  </si>
-  <si>
     <t>[Inserm U1283 / CNRS 8199](http://www.good.cnrs.fr/?lang=en)</t>
   </si>
   <si>
@@ -711,6 +708,9 @@
   </si>
   <si>
     <t>Head of Biostatistics (Institut Pasteur de Lille)</t>
+  </si>
+  <si>
+    <t>https://mickael.canouil.fr/</t>
   </si>
 </sst>
 </file>
@@ -1044,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,10 +1099,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -1114,7 +1114,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="G2" t="s">
         <v>132</v>
@@ -1129,7 +1129,7 @@
         <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1266,7 +1266,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1579,7 +1579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>167</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>167</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>187</v>
@@ -2287,7 +2287,7 @@
         <v>151</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
feat: update with new job and picture
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profils\mcanouil\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcanouil/Projects/perso/curriculum-vitae/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC643FFA-CFE9-ED48-8FC1-C059BD0D76B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="207">
   <si>
     <t>position</t>
   </si>
@@ -64,12 +65,6 @@
   </si>
   <si>
     <t>Lille, France</t>
-  </si>
-  <si>
-    <t>mickael.canouil@cnrs.fr</t>
-  </si>
-  <si>
-    <t>+33 (0)3 74 00 81 29</t>
   </si>
   <si>
     <t>mickaelcanouil</t>
@@ -615,20 +610,11 @@
     <t>website</t>
   </si>
   <si>
-    <t>[Inserm U1283 / CNRS 8199](http://www.good.cnrs.fr/?lang=en)</t>
-  </si>
-  <si>
     <t>[R Lille - R User Group (rlille.fr)](https://rlille.fr/)</t>
   </si>
   <si>
     <t>A Statistical Seminar Applied on Type 2 Diabetes  
 (Host: Pr. Paul Franks)</t>
-  </si>
-  <si>
-    <t>Head of Biostatistics</t>
-  </si>
-  <si>
-    <t>I'm currently working for the *Institut Pasteur de Lille* at the *Inserm U1283 / CNRS UMR 8199 - "Functional (Epi)genomics and Molecular Physiology of Diabetes and Related Diseases"* as *Head of Biostatistics*.</t>
   </si>
   <si>
     <t>Head of Biostatistics (CNRS)</t>
@@ -667,11 +653,49 @@
   <si>
     <t>Thirty minutes overview (in English)</t>
   </si>
+  <si>
+    <t>I am currently working as a consultant in **Biostatistics** in the field of genetics,
+*i.e.*, proteomics, metabolomics, transcriptomics, *etc.*
+in Lille &amp; Paris, France.</t>
+  </si>
+  <si>
+    <t>Consulting Senior Biostatistician</t>
+  </si>
+  <si>
+    <t>Consulting Senior Biostatistician (IT&amp;M Stats)</t>
+  </si>
+  <si>
+    <t>Oct. 2022</t>
+  </si>
+  <si>
+    <t>Nov. 2022</t>
+  </si>
+  <si>
+    <t>L'Oréal</t>
+  </si>
+  <si>
+    <t>Statistical analyses of lipidomics and microbiome data</t>
+  </si>
+  <si>
+    <t>[IT&amp;M Stats](https://it-m.fr/nos-filiales/itm-stats/)</t>
+  </si>
+  <si>
+    <t>pro@mickael.canouil.dev</t>
+  </si>
+  <si>
+    <t>MickaelCanouil</t>
+  </si>
+  <si>
+    <t>mastodon</t>
+  </si>
+  <si>
+    <t>MickaelCanouil@fosstodon.org</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -710,15 +734,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -996,28 +1021,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1034,10 +1060,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1049,42 +1075,45 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="L1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
       <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
-        <v>185</v>
+        <v>204</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="L2" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1093,90 +1122,90 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
         <v>110</v>
       </c>
-      <c r="C2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1185,51 +1214,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="67.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="67.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1238,43 +1267,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1286,153 +1315,153 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1441,88 +1470,88 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="142.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="142.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
         <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1531,24 +1560,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="117.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="117.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1559,153 +1588,173 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>55</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>56</v>
       </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
         <v>47</v>
       </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>198</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1714,156 +1763,156 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="131" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1872,183 +1921,183 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>79</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
         <v>140</v>
       </c>
-      <c r="E2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" t="s">
         <v>82</v>
       </c>
-      <c r="C4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" t="s">
         <v>141</v>
       </c>
-      <c r="B6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C7" t="s">
-        <v>143</v>
-      </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2058,24 +2107,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="99.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="99.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2084,33 +2133,33 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" t="s">
         <v>95</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" t="s">
-        <v>97</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2119,138 +2168,138 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" customWidth="1"/>
+    <col min="1" max="1" width="54.6640625" customWidth="1"/>
     <col min="2" max="2" width="85" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" display="https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility-french/"/>
-    <hyperlink ref="E7" r:id="rId2" display="https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility/"/>
+    <hyperlink ref="E6" r:id="rId1" display="https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility-french/" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="E7" r:id="rId2" display="https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility/" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
feat: update with new job and picture (#9)
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profils\mcanouil\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcanouil/Projects/perso/curriculum-vitae/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC643FFA-CFE9-ED48-8FC1-C059BD0D76B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="207">
   <si>
     <t>position</t>
   </si>
@@ -64,12 +65,6 @@
   </si>
   <si>
     <t>Lille, France</t>
-  </si>
-  <si>
-    <t>mickael.canouil@cnrs.fr</t>
-  </si>
-  <si>
-    <t>+33 (0)3 74 00 81 29</t>
   </si>
   <si>
     <t>mickaelcanouil</t>
@@ -615,20 +610,11 @@
     <t>website</t>
   </si>
   <si>
-    <t>[Inserm U1283 / CNRS 8199](http://www.good.cnrs.fr/?lang=en)</t>
-  </si>
-  <si>
     <t>[R Lille - R User Group (rlille.fr)](https://rlille.fr/)</t>
   </si>
   <si>
     <t>A Statistical Seminar Applied on Type 2 Diabetes  
 (Host: Pr. Paul Franks)</t>
-  </si>
-  <si>
-    <t>Head of Biostatistics</t>
-  </si>
-  <si>
-    <t>I'm currently working for the *Institut Pasteur de Lille* at the *Inserm U1283 / CNRS UMR 8199 - "Functional (Epi)genomics and Molecular Physiology of Diabetes and Related Diseases"* as *Head of Biostatistics*.</t>
   </si>
   <si>
     <t>Head of Biostatistics (CNRS)</t>
@@ -667,11 +653,49 @@
   <si>
     <t>Thirty minutes overview (in English)</t>
   </si>
+  <si>
+    <t>I am currently working as a consultant in **Biostatistics** in the field of genetics,
+*i.e.*, proteomics, metabolomics, transcriptomics, *etc.*
+in Lille &amp; Paris, France.</t>
+  </si>
+  <si>
+    <t>Consulting Senior Biostatistician</t>
+  </si>
+  <si>
+    <t>Consulting Senior Biostatistician (IT&amp;M Stats)</t>
+  </si>
+  <si>
+    <t>Oct. 2022</t>
+  </si>
+  <si>
+    <t>Nov. 2022</t>
+  </si>
+  <si>
+    <t>L'Oréal</t>
+  </si>
+  <si>
+    <t>Statistical analyses of lipidomics and microbiome data</t>
+  </si>
+  <si>
+    <t>[IT&amp;M Stats](https://it-m.fr/nos-filiales/itm-stats/)</t>
+  </si>
+  <si>
+    <t>pro@mickael.canouil.dev</t>
+  </si>
+  <si>
+    <t>MickaelCanouil</t>
+  </si>
+  <si>
+    <t>mastodon</t>
+  </si>
+  <si>
+    <t>MickaelCanouil@fosstodon.org</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -710,15 +734,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -996,28 +1021,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1034,10 +1060,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1049,42 +1075,45 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="L1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
       <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
-        <v>185</v>
+        <v>204</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="L2" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1093,90 +1122,90 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
         <v>110</v>
       </c>
-      <c r="C2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1185,51 +1214,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="67.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="67.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1238,43 +1267,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1286,153 +1315,153 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1441,88 +1470,88 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="142.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="142.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
         <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1531,24 +1560,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="117.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="117.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1559,153 +1588,173 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>55</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>56</v>
       </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
         <v>47</v>
       </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>198</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1714,156 +1763,156 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="131" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1872,183 +1921,183 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>79</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
         <v>140</v>
       </c>
-      <c r="E2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" t="s">
         <v>82</v>
       </c>
-      <c r="C4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" t="s">
         <v>141</v>
       </c>
-      <c r="B6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C7" t="s">
-        <v>143</v>
-      </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2058,24 +2107,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="99.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="99.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2084,33 +2133,33 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" t="s">
         <v>95</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" t="s">
-        <v>97</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2119,138 +2168,138 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" customWidth="1"/>
+    <col min="1" max="1" width="54.6640625" customWidth="1"/>
     <col min="2" max="2" width="85" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" display="https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility-french/"/>
-    <hyperlink ref="E7" r:id="rId2" display="https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility/"/>
+    <hyperlink ref="E6" r:id="rId1" display="https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility-french/" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="E7" r:id="rId2" display="https://mickael.canouil.fr/talk/my-journey-to-transparency-and-reproducibility/" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>